<commit_message>
feat: contamination, dioxin_like, change graph relative to norm value, add general evaluation
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/dioxine_like/general_eval_dioxine_like_TEQ.xlsx
+++ b/inst/results/data_contam/dioxine_like/general_eval_dioxine_like_TEQ.xlsx
@@ -398,7 +398,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>↑  ↓  red</t>
+          <t>↑  ↓  orange</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>red</t>
+          <t>orange</t>
         </is>
       </c>
     </row>

</xml_diff>